<commit_message>
TB-775 TB-747 fix test steps
</commit_message>
<xml_diff>
--- a/jems-ui/e2e/cypress/fixtures/programme/TB-747-project-export-de-de.xlsx
+++ b/jems-ui/e2e/cypress/fixtures/programme/TB-747-project-export-de-de.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jems\ems\jems-ui\e2e\cypress\fixtures\programme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E826AB8-15BD-4228-830C-1F03261A0344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD01D7D-4D14-405C-AFB8-3843E3F0BFA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="36105" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="750" yWindow="7155" windowWidth="50250" windowHeight="6765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project data" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="136">
-  <si>
-    <t>Cypress automated environment - project data - 2022.12.02 - 13:37:11</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="135">
   <si>
     <t>Project id (automatically created)</t>
   </si>
@@ -401,9 +398,6 @@
     <t>Explanatory notes</t>
   </si>
   <si>
-    <t>Contracted On</t>
-  </si>
-  <si>
     <t>ERDF DE</t>
   </si>
   <si>
@@ -429,6 +423,9 @@
   </si>
   <si>
     <t>% of total Other fund DE</t>
+  </si>
+  <si>
+    <t>Contracted (entry into force)</t>
   </si>
 </sst>
 </file>
@@ -977,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CW7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CG1" workbookViewId="0">
-      <selection activeCell="CI7" sqref="CI7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="CW4" sqref="CW4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,312 +1077,312 @@
     <col min="98" max="98" width="23.42578125" customWidth="1"/>
     <col min="99" max="99" width="25" customWidth="1"/>
     <col min="100" max="100" width="21.42578125" customWidth="1"/>
-    <col min="101" max="101" width="14.140625" customWidth="1"/>
+    <col min="101" max="101" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:101" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="D1" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="E1" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="23" t="s">
+      <c r="J1" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="K1" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="M1" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="N1" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="O1" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="P1" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="S1" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q1" s="23" t="s">
+      <c r="T1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="V1" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="W1" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="S1" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="T1" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="U1" s="23" t="s">
+      <c r="X1" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="V1" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="W1" s="23" t="s">
+      <c r="Z1" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA1" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB1" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC1" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD1" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE1" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF1" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG1" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH1" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI1" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ1" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK1" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="X1" s="23" t="s">
+      <c r="AL1" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="Y1" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z1" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA1" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB1" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC1" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD1" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE1" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF1" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="AG1" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="AH1" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="AI1" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ1" s="23" t="s">
+      <c r="AM1" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="AN1" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="AK1" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="AL1" s="23" t="s">
+      <c r="AO1" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP1" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ1" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR1" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS1" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="AT1" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="AU1" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="AV1" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW1" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX1" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="AY1" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ1" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA1" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB1" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="BC1" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="BD1" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="BE1" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF1" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="BG1" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="BH1" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="BI1" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="BJ1" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="BK1" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="BL1" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="BM1" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="BN1" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="BO1" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="BP1" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="BQ1" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="BR1" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="BS1" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="BT1" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="BU1" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="BV1" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="BW1" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="BX1" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="BY1" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ1" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="CA1" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="CB1" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="CC1" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="CD1" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="CE1" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="CF1" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="CG1" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="CH1" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="CI1" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="CJ1" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="CK1" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="CL1" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="CM1" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="CN1" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="CO1" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="CP1" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="CQ1" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="CR1" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="CS1" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="CT1" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="CU1" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="CV1" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="CW1" s="25" t="s">
         <v>134</v>
-      </c>
-      <c r="AM1" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="AN1" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="AO1" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP1" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="AQ1" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="AR1" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="AS1" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="AT1" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="AU1" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="AV1" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="AW1" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="AX1" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="AY1" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="AZ1" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="BA1" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="BB1" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="BC1" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="BD1" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="BE1" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="BF1" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="BG1" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="BH1" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="BI1" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="BJ1" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="BK1" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL1" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="BM1" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="BN1" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="BO1" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="BP1" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="BQ1" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="BR1" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="BS1" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="BT1" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="BU1" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="BV1" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="BW1" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="BX1" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="BY1" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="BZ1" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="CA1" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="CB1" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="CC1" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="CD1" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="CE1" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="CF1" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="CG1" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="CH1" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="CI1" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="CJ1" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="CK1" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="CL1" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="CM1" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="CN1" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="CO1" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="CP1" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="CQ1" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="CR1" s="24" t="s">
-        <v>120</v>
-      </c>
-      <c r="CS1" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="CT1" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="CU1" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="CV1" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="CW1" s="25" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:101" x14ac:dyDescent="0.25">
@@ -1400,19 +1397,19 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="N2" s="5">
         <v>24</v>
@@ -1604,19 +1601,19 @@
         <v>900.16</v>
       </c>
       <c r="BY2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="BZ2" s="5" t="s">
+      <c r="CA2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="CA2" s="5" t="s">
+      <c r="CB2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="CB2" s="5" t="s">
+      <c r="CC2" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="CC2" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="CD2" s="5"/>
       <c r="CE2" s="7"/>
@@ -1630,28 +1627,28 @@
       <c r="CM2" s="8"/>
       <c r="CN2" s="8"/>
       <c r="CO2" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="CP2" s="9">
         <v>44630</v>
       </c>
       <c r="CQ2" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CR2" s="9">
         <v>44630</v>
       </c>
       <c r="CS2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="CT2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="CT2" s="8" t="s">
+      <c r="CU2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="CU2" s="8" t="s">
+      <c r="CV2" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="CV2" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="CW2" s="10"/>
     </row>
@@ -1667,19 +1664,19 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="N3" s="5">
         <v>24</v>
@@ -1871,19 +1868,19 @@
         <v>900.16</v>
       </c>
       <c r="BY3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="BZ3" s="5" t="s">
+      <c r="CA3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="CA3" s="5" t="s">
+      <c r="CB3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="CB3" s="5" t="s">
+      <c r="CC3" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="CC3" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="CD3" s="5"/>
       <c r="CE3" s="7"/>
@@ -1897,28 +1894,28 @@
       <c r="CM3" s="8"/>
       <c r="CN3" s="8"/>
       <c r="CO3" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="CP3" s="9">
         <v>44630</v>
       </c>
       <c r="CQ3" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CR3" s="9">
         <v>44630</v>
       </c>
       <c r="CS3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="CT3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="CT3" s="8" t="s">
+      <c r="CU3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="CU3" s="8" t="s">
+      <c r="CV3" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="CV3" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="CW3" s="10"/>
     </row>
@@ -1934,19 +1931,19 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="N4" s="5">
         <v>24</v>
@@ -2138,19 +2135,19 @@
         <v>900.16</v>
       </c>
       <c r="BY4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="BZ4" s="5" t="s">
+      <c r="CA4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="CA4" s="5" t="s">
+      <c r="CB4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="CB4" s="5" t="s">
+      <c r="CC4" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="CC4" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="CD4" s="5"/>
       <c r="CE4" s="7"/>
@@ -2164,28 +2161,28 @@
       <c r="CM4" s="8"/>
       <c r="CN4" s="8"/>
       <c r="CO4" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="CP4" s="9">
         <v>44630</v>
       </c>
       <c r="CQ4" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CR4" s="9">
         <v>44630</v>
       </c>
       <c r="CS4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="CT4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="CT4" s="8" t="s">
+      <c r="CU4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="CU4" s="8" t="s">
+      <c r="CV4" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="CV4" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="CW4" s="10"/>
     </row>
@@ -2201,19 +2198,19 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="N5" s="5">
         <v>24</v>
@@ -2405,19 +2402,19 @@
         <v>900.16</v>
       </c>
       <c r="BY5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="BZ5" s="5" t="s">
+      <c r="CA5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="CA5" s="5" t="s">
+      <c r="CB5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="CB5" s="5" t="s">
+      <c r="CC5" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="CC5" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="CD5" s="5"/>
       <c r="CE5" s="7"/>
@@ -2431,28 +2428,28 @@
       <c r="CM5" s="8"/>
       <c r="CN5" s="8"/>
       <c r="CO5" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="CP5" s="9">
         <v>44630</v>
       </c>
       <c r="CQ5" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CR5" s="9">
         <v>44630</v>
       </c>
       <c r="CS5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="CT5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="CT5" s="8" t="s">
+      <c r="CU5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="CU5" s="8" t="s">
+      <c r="CV5" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="CV5" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="CW5" s="10"/>
     </row>
@@ -2468,19 +2465,19 @@
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="K6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="N6" s="5">
         <v>24</v>
@@ -2672,19 +2669,19 @@
         <v>900.16</v>
       </c>
       <c r="BY6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="BZ6" s="5" t="s">
+      <c r="CA6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="CA6" s="5" t="s">
+      <c r="CB6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="CB6" s="5" t="s">
+      <c r="CC6" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="CC6" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="CD6" s="5"/>
       <c r="CE6" s="7"/>
@@ -2698,28 +2695,28 @@
       <c r="CM6" s="8"/>
       <c r="CN6" s="8"/>
       <c r="CO6" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="CP6" s="9">
         <v>44630</v>
       </c>
       <c r="CQ6" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CR6" s="9">
         <v>44630</v>
       </c>
       <c r="CS6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="CT6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="CT6" s="8" t="s">
+      <c r="CU6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="CU6" s="8" t="s">
+      <c r="CV6" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="CV6" s="8" t="s">
-        <v>17</v>
       </c>
       <c r="CW6" s="10"/>
     </row>
@@ -2735,19 +2732,19 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="K7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="L7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="14" t="s">
+      <c r="M7" s="14" t="s">
         <v>6</v>
-      </c>
-      <c r="M7" s="14" t="s">
-        <v>7</v>
       </c>
       <c r="N7" s="14">
         <v>24</v>
@@ -2939,19 +2936,19 @@
         <v>900.16</v>
       </c>
       <c r="BY7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="BZ7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="BZ7" s="14" t="s">
+      <c r="CA7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="CA7" s="14" t="s">
+      <c r="CB7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="CB7" s="14" t="s">
+      <c r="CC7" s="14" t="s">
         <v>11</v>
-      </c>
-      <c r="CC7" s="14" t="s">
-        <v>12</v>
       </c>
       <c r="CD7" s="14"/>
       <c r="CE7" s="16"/>
@@ -2965,28 +2962,28 @@
       <c r="CM7" s="17"/>
       <c r="CN7" s="17"/>
       <c r="CO7" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="CP7" s="18">
         <v>44630</v>
       </c>
       <c r="CQ7" s="17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="CR7" s="18">
         <v>44630</v>
       </c>
       <c r="CS7" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="CT7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="CT7" s="17" t="s">
+      <c r="CU7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="CU7" s="17" t="s">
+      <c r="CV7" s="17" t="s">
         <v>16</v>
-      </c>
-      <c r="CV7" s="17" t="s">
-        <v>17</v>
       </c>
       <c r="CW7" s="19"/>
     </row>
@@ -2999,7 +2996,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3030,82 +3029,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>2</v>
-      </c>
       <c r="C2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="E2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="F2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="G2" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="H2" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="I2" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="J2" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="K2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="L2" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="M2" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="N2" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="O2" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="20" t="s">
+      <c r="P2" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="20" t="s">
+      <c r="Q2" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="20" t="s">
+      <c r="R2" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="R2" s="20" t="s">
+      <c r="S2" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="S2" s="20" t="s">
+      <c r="T2" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="T2" s="20" t="s">
+      <c r="U2" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="20" t="s">
+      <c r="V2" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="V2" s="20" t="s">
+      <c r="W2" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="20" t="s">
+      <c r="X2" s="20" t="s">
         <v>38</v>
-      </c>
-      <c r="X2" s="20" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>